<commit_message>
revisi EP04: Kajian Resep dan Pemberian Obat
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4455,9 +4455,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
@@ -4556,15 +4556,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4578,30 +4570,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4615,9 +4593,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4638,8 +4615,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4655,15 +4633,38 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4677,29 +4678,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4750,31 +4750,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4786,7 +4768,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4804,61 +4792,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4876,13 +4822,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4894,13 +4894,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4912,19 +4918,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5057,6 +5051,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -5068,6 +5071,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5087,33 +5110,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -5125,6 +5121,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5143,162 +5148,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7718,7 +7712,7 @@
   <dimension ref="A1:G373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11289,7 +11283,7 @@
       <c r="A217" s="111" t="s">
         <v>499</v>
       </c>
-      <c r="B217" s="41" t="s">
+      <c r="B217" s="73" t="s">
         <v>815</v>
       </c>
       <c r="C217" s="52" t="s">

</xml_diff>

<commit_message>
revisi SOP pemberian informasi obat PIO
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4454,11 +4454,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -4555,46 +4555,32 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4609,7 +4595,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4624,8 +4631,16 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4647,38 +4662,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4692,8 +4684,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4750,7 +4750,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4762,19 +4840,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4786,91 +4888,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4888,7 +4906,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4900,25 +4918,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5051,15 +5051,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -5075,11 +5066,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5110,17 +5107,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5151,148 +5151,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5488,10 +5488,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -7712,7 +7712,7 @@
   <dimension ref="A1:G373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219"/>
+      <selection activeCell="B218" sqref="B218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11301,7 +11301,7 @@
       <c r="A218" s="111" t="s">
         <v>501</v>
       </c>
-      <c r="B218" s="41" t="s">
+      <c r="B218" s="73" t="s">
         <v>817</v>
       </c>
       <c r="C218" s="52" t="s">

</xml_diff>

<commit_message>
revisi EP06: SOP Penyediaan dan Penyimpanan Obat Emergensi
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22770" windowHeight="12540" activeTab="1"/>
+    <workbookView windowWidth="27795" windowHeight="12540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SK BAB I-V" sheetId="1" r:id="rId1"/>
@@ -4454,11 +4454,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -4564,7 +4564,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4586,30 +4618,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4624,46 +4634,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4678,17 +4649,46 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4750,19 +4750,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4774,7 +4762,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4792,7 +4786,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4810,60 +4828,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -4876,13 +4840,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4894,25 +4876,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4925,6 +4919,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5051,6 +5051,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -5077,6 +5086,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5110,8 +5134,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5120,173 +5144,149 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5488,10 +5488,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -7711,8 +7711,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="B218" sqref="B218"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11319,7 +11319,7 @@
       <c r="A219" s="111" t="s">
         <v>503</v>
       </c>
-      <c r="B219" s="41" t="s">
+      <c r="B219" s="73" t="s">
         <v>819</v>
       </c>
       <c r="C219" s="52" t="s">

</xml_diff>

<commit_message>
revisi EP06: SOP Monitoring Penyediaan Obat Emergensi
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4454,11 +4454,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -4555,14 +4555,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -4578,11 +4570,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4594,32 +4585,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4634,14 +4601,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4664,7 +4632,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4672,7 +4640,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4692,10 +4667,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4750,13 +4750,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4768,7 +4780,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4786,7 +4804,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4798,133 +4918,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5075,6 +5075,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -5116,21 +5131,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -5151,148 +5151,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7712,7 +7712,7 @@
   <dimension ref="A1:G373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219"/>
+      <selection activeCell="B220" sqref="B220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11337,7 +11337,7 @@
       <c r="A220" s="111" t="s">
         <v>505</v>
       </c>
-      <c r="B220" s="41" t="s">
+      <c r="B220" s="73" t="s">
         <v>821</v>
       </c>
       <c r="C220" s="52" t="s">

</xml_diff>

<commit_message>
contreng warna SOP MESO sudah
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4462,11 +4462,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -4557,33 +4557,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -4593,7 +4566,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4615,16 +4600,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4639,29 +4638,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4675,6 +4652,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -4682,8 +4667,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4697,9 +4683,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4762,7 +4762,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4774,49 +4870,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4828,13 +4924,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4852,97 +4942,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5043,10 +5043,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -5055,8 +5053,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5100,6 +5098,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5129,149 +5138,140 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -7688,7 +7688,7 @@
   <dimension ref="A1:G373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="B226" sqref="B226"/>
+      <selection activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11587,7 +11587,7 @@
       <c r="A237" s="46" t="s">
         <v>541</v>
       </c>
-      <c r="B237" s="55" t="s">
+      <c r="B237" s="65" t="s">
         <v>855</v>
       </c>
       <c r="C237" s="46" t="s">

</xml_diff>

<commit_message>
new SOP: PTO; edit SOP: SOP Penyimpanan Obat dan BMHP
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4461,12 +4461,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -4549,127 +4549,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4686,6 +4573,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -4699,7 +4594,112 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4762,7 +4762,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4774,25 +4834,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4804,7 +4870,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4816,37 +4900,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4858,91 +4936,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5041,20 +5041,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5064,6 +5061,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5083,27 +5095,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -5124,155 +5119,160 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5448,10 +5448,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5515,7 +5515,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7687,8 +7687,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="B237" sqref="B237"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="B238" sqref="B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11603,7 +11603,7 @@
       <c r="A238" s="46" t="s">
         <v>543</v>
       </c>
-      <c r="B238" s="55" t="s">
+      <c r="B238" s="65" t="s">
         <v>857</v>
       </c>
       <c r="C238" s="46" t="s">

</xml_diff>

<commit_message>
new SOP: SOP Pemusnahan resep
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4462,11 +4462,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -4549,9 +4549,27 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -4571,6 +4589,26 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -4578,7 +4616,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -4593,13 +4631,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -4608,17 +4639,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4637,22 +4669,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -4660,8 +4676,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4674,32 +4691,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4762,19 +4762,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4786,25 +4786,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4822,85 +4810,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4918,7 +4834,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4930,19 +4888,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5041,6 +5041,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5066,21 +5075,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -5095,11 +5089,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5121,15 +5121,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -5138,145 +5129,154 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5440,6 +5440,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5917,37 +5920,37 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="5.5" style="40" customWidth="1"/>
-    <col min="2" max="2" width="59.5" style="74" customWidth="1"/>
-    <col min="3" max="3" width="19.6166666666667" style="75" customWidth="1"/>
-    <col min="4" max="4" width="18.8666666666667" style="75" customWidth="1"/>
+    <col min="2" max="2" width="59.5" style="75" customWidth="1"/>
+    <col min="3" max="3" width="19.6166666666667" style="76" customWidth="1"/>
+    <col min="4" max="4" width="18.8666666666667" style="76" customWidth="1"/>
     <col min="5" max="5" width="18.8666666666667" style="40" customWidth="1"/>
     <col min="6" max="1024" width="9" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" s="71" customFormat="1" ht="12" customHeight="1" spans="1:5">
-      <c r="A1" s="76" t="s">
+    <row r="1" s="72" customFormat="1" ht="12" customHeight="1" spans="1:5">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-    </row>
-    <row r="2" s="71" customFormat="1" ht="12" customHeight="1" spans="1:5">
-      <c r="A2" s="76" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+    </row>
+    <row r="2" s="72" customFormat="1" ht="12" customHeight="1" spans="1:5">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
     </row>
     <row r="3" ht="17.25" spans="1:5">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="77"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
     </row>
     <row r="4" ht="31.5" customHeight="1" spans="1:5">
       <c r="A4" s="39" t="s">
@@ -5956,7 +5959,7 @@
       <c r="B4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="81" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="39" t="s">
@@ -5967,1706 +5970,1706 @@
       </c>
     </row>
     <row r="5" ht="21" customHeight="1" spans="1:5">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="81"/>
+      <c r="E5" s="82"/>
     </row>
     <row r="6" ht="21" customHeight="1" spans="1:5">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="82" t="s">
+      <c r="B6" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="83" t="s">
+      <c r="D6" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="81"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" ht="21" customHeight="1" spans="1:5">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="83" t="s">
+      <c r="D7" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="81"/>
+      <c r="E7" s="82"/>
     </row>
     <row r="8" ht="32.25" customHeight="1" spans="1:5">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="83" t="s">
+      <c r="D8" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="82" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" ht="32.25" customHeight="1" spans="1:5">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="82" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" ht="21" customHeight="1" spans="1:5">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="81" t="s">
+      <c r="C10" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="81"/>
+      <c r="E10" s="82"/>
     </row>
     <row r="11" ht="21" customHeight="1" spans="1:5">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="81" t="s">
+      <c r="E11" s="82" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" ht="33.75" customHeight="1" spans="1:5">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="81" t="s">
+      <c r="C12" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="81" t="s">
+      <c r="E12" s="82" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" ht="21" customHeight="1" spans="1:5">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="83" t="s">
+      <c r="D13" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="81" t="s">
+      <c r="E13" s="82" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" ht="21" customHeight="1" spans="1:5">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="82" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D14" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="81"/>
+      <c r="E14" s="82"/>
     </row>
     <row r="15" ht="32.25" customHeight="1" spans="1:5">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="84" t="s">
+      <c r="B15" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="81"/>
+      <c r="E15" s="82"/>
     </row>
     <row r="16" s="13" customFormat="1" ht="48.75" customHeight="1" spans="1:5">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="81" t="s">
+      <c r="C16" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="83" t="s">
+      <c r="D16" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="81" t="s">
+      <c r="E16" s="82" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" ht="21" customHeight="1" spans="1:5">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="83" t="s">
+      <c r="D17" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="81" t="s">
+      <c r="E17" s="82" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" ht="21" customHeight="1" spans="1:5">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="85" t="s">
+      <c r="B18" s="86" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="83" t="s">
+      <c r="D18" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="81"/>
+      <c r="E18" s="82"/>
     </row>
     <row r="19" ht="21" customHeight="1" spans="1:5">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="81" t="s">
+      <c r="C19" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="83" t="s">
+      <c r="D19" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="81"/>
+      <c r="E19" s="82"/>
     </row>
     <row r="20" ht="21" customHeight="1" spans="1:5">
-      <c r="A20" s="81" t="s">
+      <c r="A20" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="81" t="s">
+      <c r="C20" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="83" t="s">
+      <c r="D20" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="81"/>
+      <c r="E20" s="82"/>
     </row>
     <row r="21" ht="21" customHeight="1" spans="1:5">
-      <c r="A21" s="81" t="s">
+      <c r="A21" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="81" t="s">
+      <c r="C21" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="83" t="s">
+      <c r="D21" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="81" t="s">
+      <c r="E21" s="82" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" ht="21" customHeight="1" spans="1:5">
-      <c r="A22" s="81" t="s">
+      <c r="A22" s="82" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="84" t="s">
+      <c r="B22" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="81" t="s">
+      <c r="C22" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="83" t="s">
+      <c r="D22" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="81"/>
+      <c r="E22" s="82"/>
     </row>
     <row r="23" ht="21" customHeight="1" spans="1:5">
-      <c r="A23" s="81" t="s">
+      <c r="A23" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="83" t="s">
+      <c r="D23" s="84" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="81"/>
+      <c r="E23" s="82"/>
     </row>
     <row r="24" ht="21" customHeight="1" spans="1:5">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="82" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="84" t="s">
+      <c r="B24" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="81" t="s">
+      <c r="C24" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="83" t="s">
+      <c r="D24" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="81" t="s">
+      <c r="E24" s="82" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="25" ht="21" customHeight="1" spans="1:5">
-      <c r="A25" s="81" t="s">
+      <c r="A25" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="85" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="81" t="s">
+      <c r="C25" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="81"/>
+      <c r="E25" s="82"/>
     </row>
     <row r="26" ht="21" customHeight="1" spans="1:5">
-      <c r="A26" s="81" t="s">
+      <c r="A26" s="82" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="84" t="s">
+      <c r="B26" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="81" t="s">
+      <c r="C26" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="81"/>
+      <c r="E26" s="82"/>
     </row>
     <row r="27" ht="21" customHeight="1" spans="1:5">
-      <c r="A27" s="81" t="s">
+      <c r="A27" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="84" t="s">
+      <c r="B27" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="81" t="s">
+      <c r="C27" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="83" t="s">
+      <c r="D27" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="81"/>
+      <c r="E27" s="82"/>
     </row>
     <row r="28" ht="21" customHeight="1" spans="1:5">
-      <c r="A28" s="81" t="s">
+      <c r="A28" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="85" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="81"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="81"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="82"/>
     </row>
     <row r="29" ht="21" customHeight="1" spans="1:5">
-      <c r="A29" s="81" t="s">
+      <c r="A29" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="B29" s="84" t="s">
+      <c r="B29" s="85" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="81" t="s">
+      <c r="C29" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="83" t="s">
+      <c r="D29" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="81" t="s">
+      <c r="E29" s="82" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="30" ht="33.75" customHeight="1" spans="1:5">
-      <c r="A30" s="81" t="s">
+      <c r="A30" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="84" t="s">
+      <c r="B30" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="81" t="s">
+      <c r="C30" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="83" t="s">
+      <c r="D30" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="81" t="s">
+      <c r="E30" s="82" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" ht="33.75" customHeight="1" spans="1:5">
-      <c r="A31" s="81" t="s">
+      <c r="A31" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="84" t="s">
+      <c r="B31" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="81" t="s">
+      <c r="C31" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="83" t="s">
+      <c r="D31" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="E31" s="81" t="s">
+      <c r="E31" s="82" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="32" ht="21" customHeight="1" spans="1:5">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="82" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="84" t="s">
+      <c r="B32" s="85" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="81" t="s">
+      <c r="C32" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="83" t="s">
+      <c r="D32" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="81" t="s">
+      <c r="E32" s="82" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="33" ht="47.25" customHeight="1" spans="1:5">
-      <c r="A33" s="81" t="s">
+      <c r="A33" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="B33" s="84" t="s">
+      <c r="B33" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="C33" s="81" t="s">
+      <c r="C33" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="83" t="s">
+      <c r="D33" s="84" t="s">
         <v>103</v>
       </c>
-      <c r="E33" s="81" t="s">
+      <c r="E33" s="82" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="34" ht="36" customHeight="1" spans="1:5">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="82" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="84" t="s">
+      <c r="B34" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="81" t="s">
+      <c r="C34" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="83" t="s">
+      <c r="D34" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="E34" s="81" t="s">
+      <c r="E34" s="82" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" ht="36" customHeight="1" spans="1:5">
-      <c r="A35" s="81" t="s">
+      <c r="A35" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="C35" s="81" t="s">
+      <c r="C35" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D35" s="83" t="s">
+      <c r="D35" s="84" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="81" t="s">
+      <c r="E35" s="82" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="36" ht="47.25" customHeight="1" spans="1:5">
-      <c r="A36" s="81" t="s">
+      <c r="A36" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="81" t="s">
+      <c r="C36" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D36" s="83" t="s">
+      <c r="D36" s="84" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="81" t="s">
+      <c r="E36" s="82" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="37" ht="21" customHeight="1" spans="1:5">
-      <c r="A37" s="81" t="s">
+      <c r="A37" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="81" t="s">
+      <c r="C37" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="83" t="s">
+      <c r="D37" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="E37" s="81" t="s">
+      <c r="E37" s="82" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="38" ht="48" customHeight="1" spans="1:5">
-      <c r="A38" s="81" t="s">
+      <c r="A38" s="82" t="s">
         <v>121</v>
       </c>
-      <c r="B38" s="84" t="s">
+      <c r="B38" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="C38" s="81" t="s">
+      <c r="C38" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D38" s="83" t="s">
+      <c r="D38" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="E38" s="81" t="s">
+      <c r="E38" s="82" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="39" ht="21" customHeight="1" spans="1:5">
-      <c r="A39" s="81" t="s">
+      <c r="A39" s="82" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="84" t="s">
+      <c r="B39" s="85" t="s">
         <v>126</v>
       </c>
-      <c r="C39" s="81" t="s">
+      <c r="C39" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="83" t="s">
+      <c r="D39" s="84" t="s">
         <v>127</v>
       </c>
-      <c r="E39" s="81" t="s">
+      <c r="E39" s="82" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="40" ht="21" customHeight="1" spans="1:5">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="82" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="85" t="s">
         <v>130</v>
       </c>
-      <c r="C40" s="81" t="s">
+      <c r="C40" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="83" t="s">
+      <c r="D40" s="84" t="s">
         <v>131</v>
       </c>
-      <c r="E40" s="81" t="s">
+      <c r="E40" s="82" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="41" ht="21" customHeight="1" spans="1:5">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="B41" s="84" t="s">
+      <c r="B41" s="85" t="s">
         <v>134</v>
       </c>
-      <c r="C41" s="81" t="s">
+      <c r="C41" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="83" t="s">
+      <c r="D41" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="E41" s="81" t="s">
+      <c r="E41" s="82" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="42" ht="21" customHeight="1" spans="1:5">
-      <c r="A42" s="81" t="s">
+      <c r="A42" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="B42" s="84" t="s">
+      <c r="B42" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="C42" s="81" t="s">
+      <c r="C42" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="83" t="s">
+      <c r="D42" s="84" t="s">
         <v>138</v>
       </c>
-      <c r="E42" s="81" t="s">
+      <c r="E42" s="82" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="43" ht="21" customHeight="1" spans="1:5">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="B43" s="84" t="s">
+      <c r="B43" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="C43" s="81" t="s">
+      <c r="C43" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="83" t="s">
+      <c r="D43" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="E43" s="81" t="s">
+      <c r="E43" s="82" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="44" ht="21" customHeight="1" spans="1:5">
-      <c r="A44" s="81" t="s">
+      <c r="A44" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="B44" s="84" t="s">
+      <c r="B44" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="81" t="s">
+      <c r="C44" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="83" t="s">
+      <c r="D44" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="E44" s="81" t="s">
+      <c r="E44" s="82" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="45" ht="36" customHeight="1" spans="1:5">
-      <c r="A45" s="81" t="s">
+      <c r="A45" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="B45" s="84" t="s">
+      <c r="B45" s="85" t="s">
         <v>148</v>
       </c>
-      <c r="C45" s="81" t="s">
+      <c r="C45" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="83" t="s">
+      <c r="D45" s="84" t="s">
         <v>149</v>
       </c>
-      <c r="E45" s="81" t="s">
+      <c r="E45" s="82" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="46" ht="21" customHeight="1" spans="1:6">
-      <c r="A46" s="81" t="s">
+      <c r="A46" s="82" t="s">
         <v>150</v>
       </c>
-      <c r="B46" s="84" t="s">
+      <c r="B46" s="85" t="s">
         <v>151</v>
       </c>
       <c r="C46" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="D46" s="83" t="s">
+      <c r="D46" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="E46" s="81" t="s">
+      <c r="E46" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="F46" s="88"/>
+      <c r="F46" s="89"/>
     </row>
     <row r="47" ht="21" customHeight="1" spans="1:6">
-      <c r="A47" s="81" t="s">
+      <c r="A47" s="82" t="s">
         <v>154</v>
       </c>
-      <c r="B47" s="84" t="s">
+      <c r="B47" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="C47" s="81" t="s">
+      <c r="C47" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="83" t="s">
+      <c r="D47" s="84" t="s">
         <v>156</v>
       </c>
-      <c r="E47" s="81" t="s">
+      <c r="E47" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="F47" s="88"/>
+      <c r="F47" s="89"/>
     </row>
     <row r="48" ht="21" customHeight="1" spans="1:6">
-      <c r="A48" s="81" t="s">
+      <c r="A48" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="B48" s="84" t="s">
+      <c r="B48" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="C48" s="81" t="s">
+      <c r="C48" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="83" t="s">
+      <c r="D48" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="E48" s="81" t="s">
+      <c r="E48" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="F48" s="88"/>
+      <c r="F48" s="89"/>
     </row>
     <row r="49" ht="21" customHeight="1" spans="1:5">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="82" t="s">
         <v>160</v>
       </c>
-      <c r="B49" s="84" t="s">
+      <c r="B49" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="81" t="s">
+      <c r="C49" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="83" t="s">
+      <c r="D49" s="84" t="s">
         <v>162</v>
       </c>
-      <c r="E49" s="81" t="s">
+      <c r="E49" s="82" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="50" ht="21" customHeight="1" spans="1:5">
-      <c r="A50" s="81" t="s">
+      <c r="A50" s="82" t="s">
         <v>164</v>
       </c>
-      <c r="B50" s="84" t="s">
+      <c r="B50" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="C50" s="81" t="s">
+      <c r="C50" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D50" s="83" t="s">
+      <c r="D50" s="84" t="s">
         <v>166</v>
       </c>
-      <c r="E50" s="81" t="s">
+      <c r="E50" s="82" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="51" ht="21" customHeight="1" spans="1:5">
-      <c r="A51" s="81" t="s">
+      <c r="A51" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="B51" s="84" t="s">
+      <c r="B51" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="C51" s="81" t="s">
+      <c r="C51" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D51" s="83" t="s">
+      <c r="D51" s="84" t="s">
         <v>170</v>
       </c>
-      <c r="E51" s="81" t="s">
+      <c r="E51" s="82" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="52" ht="21" customHeight="1" spans="1:5">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="B52" s="84" t="s">
+      <c r="B52" s="85" t="s">
         <v>173</v>
       </c>
-      <c r="C52" s="81" t="s">
+      <c r="C52" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="83" t="s">
+      <c r="D52" s="84" t="s">
         <v>174</v>
       </c>
-      <c r="E52" s="81" t="s">
+      <c r="E52" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="53" ht="21" customHeight="1" spans="1:5">
-      <c r="A53" s="81" t="s">
+      <c r="A53" s="82" t="s">
         <v>176</v>
       </c>
-      <c r="B53" s="84" t="s">
+      <c r="B53" s="85" t="s">
         <v>177</v>
       </c>
-      <c r="C53" s="81" t="s">
+      <c r="C53" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="83" t="s">
+      <c r="D53" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="E53" s="81" t="s">
+      <c r="E53" s="82" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="54" ht="21" customHeight="1" spans="1:5">
-      <c r="A54" s="81" t="s">
+      <c r="A54" s="82" t="s">
         <v>180</v>
       </c>
-      <c r="B54" s="84" t="s">
+      <c r="B54" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="C54" s="81" t="s">
+      <c r="C54" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D54" s="83" t="s">
+      <c r="D54" s="84" t="s">
         <v>182</v>
       </c>
-      <c r="E54" s="81" t="s">
+      <c r="E54" s="82" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="55" ht="21" customHeight="1" spans="1:5">
-      <c r="A55" s="81" t="s">
+      <c r="A55" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="B55" s="82" t="s">
+      <c r="B55" s="83" t="s">
         <v>185</v>
       </c>
-      <c r="C55" s="81" t="s">
+      <c r="C55" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="83" t="s">
+      <c r="D55" s="84" t="s">
         <v>186</v>
       </c>
-      <c r="E55" s="81"/>
+      <c r="E55" s="82"/>
     </row>
     <row r="56" ht="21" customHeight="1" spans="1:5">
-      <c r="A56" s="81" t="s">
+      <c r="A56" s="82" t="s">
         <v>187</v>
       </c>
-      <c r="B56" s="82" t="s">
+      <c r="B56" s="83" t="s">
         <v>188</v>
       </c>
-      <c r="C56" s="81" t="s">
+      <c r="C56" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D56" s="83" t="s">
+      <c r="D56" s="84" t="s">
         <v>189</v>
       </c>
-      <c r="E56" s="81"/>
+      <c r="E56" s="82"/>
     </row>
     <row r="57" ht="21" customHeight="1" spans="1:5">
-      <c r="A57" s="81" t="s">
+      <c r="A57" s="82" t="s">
         <v>190</v>
       </c>
-      <c r="B57" s="82" t="s">
+      <c r="B57" s="83" t="s">
         <v>191</v>
       </c>
-      <c r="C57" s="81" t="s">
+      <c r="C57" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="83" t="s">
+      <c r="D57" s="84" t="s">
         <v>192</v>
       </c>
-      <c r="E57" s="81"/>
+      <c r="E57" s="82"/>
     </row>
     <row r="58" ht="21" customHeight="1" spans="1:6">
-      <c r="A58" s="81" t="s">
+      <c r="A58" s="82" t="s">
         <v>193</v>
       </c>
-      <c r="B58" s="84" t="s">
+      <c r="B58" s="85" t="s">
         <v>194</v>
       </c>
-      <c r="C58" s="81" t="s">
-        <v>195</v>
-      </c>
-      <c r="D58" s="83" t="s">
+      <c r="C58" s="82" t="s">
+        <v>195</v>
+      </c>
+      <c r="D58" s="84" t="s">
         <v>196</v>
       </c>
-      <c r="E58" s="81" t="s">
+      <c r="E58" s="82" t="s">
         <v>197</v>
       </c>
-      <c r="F58" s="88"/>
+      <c r="F58" s="89"/>
     </row>
     <row r="59" ht="21" customHeight="1" spans="1:5">
-      <c r="A59" s="81" t="s">
+      <c r="A59" s="82" t="s">
         <v>198</v>
       </c>
-      <c r="B59" s="84" t="s">
+      <c r="B59" s="85" t="s">
         <v>199</v>
       </c>
-      <c r="C59" s="81" t="s">
+      <c r="C59" s="82" t="s">
         <v>200</v>
       </c>
-      <c r="D59" s="83" t="s">
+      <c r="D59" s="84" t="s">
         <v>201</v>
       </c>
-      <c r="E59" s="81" t="s">
+      <c r="E59" s="82" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="60" ht="21" customHeight="1" spans="1:5">
-      <c r="A60" s="81" t="s">
+      <c r="A60" s="82" t="s">
         <v>203</v>
       </c>
-      <c r="B60" s="84" t="s">
+      <c r="B60" s="85" t="s">
         <v>204</v>
       </c>
-      <c r="C60" s="81" t="s">
+      <c r="C60" s="82" t="s">
         <v>205</v>
       </c>
-      <c r="D60" s="83" t="s">
+      <c r="D60" s="84" t="s">
         <v>206</v>
       </c>
-      <c r="E60" s="81" t="s">
+      <c r="E60" s="82" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="61" ht="21" customHeight="1" spans="1:5">
-      <c r="A61" s="81" t="s">
+      <c r="A61" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="B61" s="84" t="s">
+      <c r="B61" s="85" t="s">
         <v>209</v>
       </c>
-      <c r="C61" s="81" t="s">
+      <c r="C61" s="82" t="s">
         <v>205</v>
       </c>
-      <c r="D61" s="83" t="s">
+      <c r="D61" s="84" t="s">
         <v>210</v>
       </c>
-      <c r="E61" s="81"/>
+      <c r="E61" s="82"/>
     </row>
     <row r="62" ht="21" customHeight="1" spans="1:5">
-      <c r="A62" s="81" t="s">
+      <c r="A62" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="B62" s="84" t="s">
+      <c r="B62" s="85" t="s">
         <v>212</v>
       </c>
-      <c r="C62" s="81" t="s">
+      <c r="C62" s="82" t="s">
         <v>205</v>
       </c>
-      <c r="D62" s="83" t="s">
+      <c r="D62" s="84" t="s">
         <v>213</v>
       </c>
-      <c r="E62" s="81"/>
+      <c r="E62" s="82"/>
     </row>
     <row r="63" ht="54" spans="1:5">
-      <c r="A63" s="81" t="s">
+      <c r="A63" s="82" t="s">
         <v>214</v>
       </c>
-      <c r="B63" s="84" t="s">
+      <c r="B63" s="85" t="s">
         <v>215</v>
       </c>
-      <c r="C63" s="87"/>
-      <c r="D63" s="83"/>
-      <c r="E63" s="81" t="s">
+      <c r="C63" s="88"/>
+      <c r="D63" s="84"/>
+      <c r="E63" s="82" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="64" ht="32.25" customHeight="1" spans="1:5">
-      <c r="A64" s="81" t="s">
+      <c r="A64" s="82" t="s">
         <v>217</v>
       </c>
-      <c r="B64" s="84" t="s">
+      <c r="B64" s="85" t="s">
         <v>218</v>
       </c>
-      <c r="C64" s="87"/>
-      <c r="D64" s="83"/>
-      <c r="E64" s="81" t="s">
+      <c r="C64" s="88"/>
+      <c r="D64" s="84"/>
+      <c r="E64" s="82" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="65" ht="36" spans="1:5">
-      <c r="A65" s="81" t="s">
+      <c r="A65" s="82" t="s">
         <v>219</v>
       </c>
-      <c r="B65" s="84" t="s">
+      <c r="B65" s="85" t="s">
         <v>220</v>
       </c>
-      <c r="C65" s="87"/>
-      <c r="D65" s="83"/>
-      <c r="E65" s="81" t="s">
+      <c r="C65" s="88"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="82" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="66" ht="33.75" customHeight="1" spans="1:5">
-      <c r="A66" s="81" t="s">
+      <c r="A66" s="82" t="s">
         <v>222</v>
       </c>
-      <c r="B66" s="84" t="s">
+      <c r="B66" s="85" t="s">
         <v>223</v>
       </c>
-      <c r="C66" s="87"/>
-      <c r="D66" s="83"/>
-      <c r="E66" s="81" t="s">
+      <c r="C66" s="88"/>
+      <c r="D66" s="84"/>
+      <c r="E66" s="82" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="67" ht="38.25" customHeight="1" spans="1:5">
-      <c r="A67" s="81" t="s">
+      <c r="A67" s="82" t="s">
         <v>224</v>
       </c>
-      <c r="B67" s="84" t="s">
+      <c r="B67" s="85" t="s">
         <v>225</v>
       </c>
-      <c r="C67" s="81" t="s">
+      <c r="C67" s="82" t="s">
         <v>226</v>
       </c>
-      <c r="D67" s="83" t="s">
+      <c r="D67" s="84" t="s">
         <v>227</v>
       </c>
-      <c r="E67" s="81" t="s">
+      <c r="E67" s="82" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="68" ht="48" customHeight="1" spans="1:5">
-      <c r="A68" s="81" t="s">
+      <c r="A68" s="82" t="s">
         <v>229</v>
       </c>
-      <c r="B68" s="84" t="s">
+      <c r="B68" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="C68" s="81" t="s">
+      <c r="C68" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="D68" s="83" t="s">
+      <c r="D68" s="84" t="s">
         <v>232</v>
       </c>
-      <c r="E68" s="81" t="s">
+      <c r="E68" s="82" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="69" ht="18" spans="1:5">
-      <c r="A69" s="81" t="s">
+      <c r="A69" s="82" t="s">
         <v>234</v>
       </c>
-      <c r="B69" s="84" t="s">
+      <c r="B69" s="85" t="s">
         <v>235</v>
       </c>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="82" t="s">
         <v>231</v>
       </c>
-      <c r="D69" s="81" t="s">
+      <c r="D69" s="82" t="s">
         <v>236</v>
       </c>
-      <c r="E69" s="81" t="s">
+      <c r="E69" s="82" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="70" s="72" customFormat="1" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A70" s="81" t="s">
+    <row r="70" s="73" customFormat="1" ht="19.5" customHeight="1" spans="1:5">
+      <c r="A70" s="82" t="s">
         <v>237</v>
       </c>
-      <c r="B70" s="82" t="s">
+      <c r="B70" s="83" t="s">
         <v>238</v>
       </c>
-      <c r="C70" s="81" t="s">
+      <c r="C70" s="82" t="s">
         <v>239</v>
       </c>
-      <c r="D70" s="81" t="s">
+      <c r="D70" s="82" t="s">
         <v>240</v>
       </c>
-      <c r="E70" s="81"/>
-    </row>
-    <row r="71" s="72" customFormat="1" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A71" s="81" t="s">
+      <c r="E70" s="82"/>
+    </row>
+    <row r="71" s="73" customFormat="1" ht="19.5" customHeight="1" spans="1:5">
+      <c r="A71" s="82" t="s">
         <v>241</v>
       </c>
-      <c r="B71" s="82" t="s">
+      <c r="B71" s="83" t="s">
         <v>242</v>
       </c>
-      <c r="C71" s="81" t="s">
+      <c r="C71" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D71" s="89" t="s">
+      <c r="D71" s="90" t="s">
         <v>244</v>
       </c>
-      <c r="E71" s="81"/>
-    </row>
-    <row r="72" s="72" customFormat="1" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A72" s="81" t="s">
+      <c r="E71" s="82"/>
+    </row>
+    <row r="72" s="73" customFormat="1" ht="19.5" customHeight="1" spans="1:5">
+      <c r="A72" s="82" t="s">
         <v>245</v>
       </c>
-      <c r="B72" s="82" t="s">
+      <c r="B72" s="83" t="s">
         <v>246</v>
       </c>
-      <c r="C72" s="81" t="s">
+      <c r="C72" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D72" s="89" t="s">
+      <c r="D72" s="90" t="s">
         <v>247</v>
       </c>
-      <c r="E72" s="81"/>
-    </row>
-    <row r="73" s="73" customFormat="1" ht="34.5" customHeight="1" spans="1:5">
-      <c r="A73" s="81" t="s">
+      <c r="E72" s="82"/>
+    </row>
+    <row r="73" s="74" customFormat="1" ht="34.5" customHeight="1" spans="1:5">
+      <c r="A73" s="82" t="s">
         <v>248</v>
       </c>
-      <c r="B73" s="84" t="s">
+      <c r="B73" s="85" t="s">
         <v>249</v>
       </c>
-      <c r="C73" s="81" t="s">
-        <v>195</v>
-      </c>
-      <c r="D73" s="89" t="s">
+      <c r="C73" s="82" t="s">
+        <v>195</v>
+      </c>
+      <c r="D73" s="90" t="s">
         <v>250</v>
       </c>
-      <c r="E73" s="81"/>
+      <c r="E73" s="82"/>
     </row>
     <row r="74" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A74" s="81" t="s">
+      <c r="A74" s="82" t="s">
         <v>251</v>
       </c>
-      <c r="B74" s="84" t="s">
+      <c r="B74" s="85" t="s">
         <v>252</v>
       </c>
-      <c r="C74" s="81" t="s">
+      <c r="C74" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D74" s="83" t="s">
+      <c r="D74" s="84" t="s">
         <v>253</v>
       </c>
-      <c r="E74" s="81"/>
+      <c r="E74" s="82"/>
     </row>
     <row r="75" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A75" s="81" t="s">
+      <c r="A75" s="82" t="s">
         <v>254</v>
       </c>
-      <c r="B75" s="86" t="s">
+      <c r="B75" s="87" t="s">
         <v>255</v>
       </c>
-      <c r="C75" s="81" t="s">
+      <c r="C75" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D75" s="83" t="s">
+      <c r="D75" s="84" t="s">
         <v>256</v>
       </c>
-      <c r="E75" s="81"/>
+      <c r="E75" s="82"/>
     </row>
     <row r="76" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A76" s="81" t="s">
+      <c r="A76" s="82" t="s">
         <v>257</v>
       </c>
-      <c r="B76" s="82" t="s">
+      <c r="B76" s="83" t="s">
         <v>258</v>
       </c>
-      <c r="C76" s="81" t="s">
+      <c r="C76" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D76" s="83" t="s">
+      <c r="D76" s="84" t="s">
         <v>259</v>
       </c>
-      <c r="E76" s="81"/>
+      <c r="E76" s="82"/>
     </row>
     <row r="77" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A77" s="81" t="s">
+      <c r="A77" s="82" t="s">
         <v>260</v>
       </c>
-      <c r="B77" s="82" t="s">
+      <c r="B77" s="83" t="s">
         <v>261</v>
       </c>
-      <c r="C77" s="81" t="s">
+      <c r="C77" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D77" s="83" t="s">
+      <c r="D77" s="84" t="s">
         <v>262</v>
       </c>
-      <c r="E77" s="81"/>
+      <c r="E77" s="82"/>
     </row>
     <row r="78" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A78" s="81" t="s">
+      <c r="A78" s="82" t="s">
         <v>263</v>
       </c>
-      <c r="B78" s="90" t="s">
+      <c r="B78" s="91" t="s">
         <v>264</v>
       </c>
-      <c r="C78" s="81" t="s">
+      <c r="C78" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D78" s="83" t="s">
+      <c r="D78" s="84" t="s">
         <v>265</v>
       </c>
-      <c r="E78" s="81"/>
+      <c r="E78" s="82"/>
     </row>
     <row r="79" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A79" s="81" t="s">
+      <c r="A79" s="82" t="s">
         <v>266</v>
       </c>
-      <c r="B79" s="90" t="s">
+      <c r="B79" s="91" t="s">
         <v>267</v>
       </c>
-      <c r="C79" s="81" t="s">
+      <c r="C79" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D79" s="91" t="s">
+      <c r="D79" s="92" t="s">
         <v>268</v>
       </c>
-      <c r="E79" s="81"/>
+      <c r="E79" s="82"/>
     </row>
     <row r="80" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A80" s="81" t="s">
+      <c r="A80" s="82" t="s">
         <v>269</v>
       </c>
-      <c r="B80" s="90" t="s">
+      <c r="B80" s="91" t="s">
         <v>270</v>
       </c>
-      <c r="C80" s="81" t="s">
+      <c r="C80" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="D80" s="91" t="s">
+      <c r="D80" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="E80" s="81"/>
+      <c r="E80" s="82"/>
     </row>
     <row r="81" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A81" s="81" t="s">
+      <c r="A81" s="82" t="s">
         <v>272</v>
       </c>
-      <c r="B81" s="82" t="s">
+      <c r="B81" s="83" t="s">
         <v>273</v>
       </c>
-      <c r="C81" s="81" t="s">
+      <c r="C81" s="82" t="s">
         <v>274</v>
       </c>
-      <c r="D81" s="91" t="s">
+      <c r="D81" s="92" t="s">
         <v>275</v>
       </c>
-      <c r="E81" s="81"/>
+      <c r="E81" s="82"/>
     </row>
     <row r="82" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A82" s="81" t="s">
+      <c r="A82" s="82" t="s">
         <v>276</v>
       </c>
-      <c r="B82" s="82" t="s">
+      <c r="B82" s="83" t="s">
         <v>277</v>
       </c>
-      <c r="C82" s="92">
+      <c r="C82" s="93">
         <v>45383</v>
       </c>
-      <c r="D82" s="91" t="s">
+      <c r="D82" s="92" t="s">
         <v>278</v>
       </c>
-      <c r="E82" s="81"/>
+      <c r="E82" s="82"/>
     </row>
     <row r="83" ht="54" spans="1:5">
-      <c r="A83" s="81" t="s">
+      <c r="A83" s="82" t="s">
         <v>279</v>
       </c>
-      <c r="B83" s="84" t="s">
+      <c r="B83" s="85" t="s">
         <v>280</v>
       </c>
-      <c r="C83" s="81"/>
-      <c r="D83" s="83"/>
-      <c r="E83" s="81" t="s">
+      <c r="C83" s="82"/>
+      <c r="D83" s="84"/>
+      <c r="E83" s="82" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="84" ht="54" spans="1:5">
-      <c r="A84" s="81" t="s">
+      <c r="A84" s="82" t="s">
         <v>282</v>
       </c>
-      <c r="B84" s="84" t="s">
+      <c r="B84" s="85" t="s">
         <v>283</v>
       </c>
-      <c r="C84" s="81"/>
-      <c r="D84" s="83"/>
-      <c r="E84" s="81" t="s">
+      <c r="C84" s="82"/>
+      <c r="D84" s="84"/>
+      <c r="E84" s="82" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="85" ht="20.25" customHeight="1" spans="1:5">
-      <c r="A85" s="81" t="s">
+      <c r="A85" s="82" t="s">
         <v>285</v>
       </c>
-      <c r="B85" s="84" t="s">
+      <c r="B85" s="85" t="s">
         <v>286</v>
       </c>
-      <c r="C85" s="81"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="81" t="s">
+      <c r="C85" s="82"/>
+      <c r="D85" s="84"/>
+      <c r="E85" s="82" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="86" ht="36" spans="1:5">
-      <c r="A86" s="81" t="s">
+      <c r="A86" s="82" t="s">
         <v>287</v>
       </c>
-      <c r="B86" s="84" t="s">
+      <c r="B86" s="85" t="s">
         <v>288</v>
       </c>
-      <c r="C86" s="81"/>
-      <c r="D86" s="83"/>
-      <c r="E86" s="81" t="s">
+      <c r="C86" s="82"/>
+      <c r="D86" s="84"/>
+      <c r="E86" s="82" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="87" ht="34.5" customHeight="1" spans="1:5">
-      <c r="A87" s="81" t="s">
+      <c r="A87" s="82" t="s">
         <v>289</v>
       </c>
-      <c r="B87" s="84" t="s">
+      <c r="B87" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="C87" s="81"/>
-      <c r="D87" s="83"/>
-      <c r="E87" s="81" t="s">
+      <c r="C87" s="82"/>
+      <c r="D87" s="84"/>
+      <c r="E87" s="82" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="88" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A88" s="81" t="s">
+      <c r="A88" s="82" t="s">
         <v>292</v>
       </c>
-      <c r="B88" s="84" t="s">
+      <c r="B88" s="85" t="s">
         <v>293</v>
       </c>
-      <c r="C88" s="81"/>
-      <c r="D88" s="83"/>
-      <c r="E88" s="81" t="s">
+      <c r="C88" s="82"/>
+      <c r="D88" s="84"/>
+      <c r="E88" s="82" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="89" ht="48.75" customHeight="1" spans="1:5">
-      <c r="A89" s="81" t="s">
+      <c r="A89" s="82" t="s">
         <v>294</v>
       </c>
-      <c r="B89" s="84" t="s">
+      <c r="B89" s="85" t="s">
         <v>295</v>
       </c>
-      <c r="C89" s="81"/>
-      <c r="D89" s="83"/>
-      <c r="E89" s="81" t="s">
+      <c r="C89" s="82"/>
+      <c r="D89" s="84"/>
+      <c r="E89" s="82" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="90" ht="18.75" customHeight="1" spans="1:5">
-      <c r="A90" s="81" t="s">
+      <c r="A90" s="82" t="s">
         <v>297</v>
       </c>
-      <c r="B90" s="84" t="s">
+      <c r="B90" s="85" t="s">
         <v>293</v>
       </c>
-      <c r="C90" s="81"/>
-      <c r="D90" s="83"/>
-      <c r="E90" s="81" t="s">
+      <c r="C90" s="82"/>
+      <c r="D90" s="84"/>
+      <c r="E90" s="82" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="91" ht="51" customHeight="1" spans="1:5">
-      <c r="A91" s="81" t="s">
+      <c r="A91" s="82" t="s">
         <v>298</v>
       </c>
-      <c r="B91" s="84" t="s">
+      <c r="B91" s="85" t="s">
         <v>299</v>
       </c>
-      <c r="C91" s="81"/>
-      <c r="D91" s="83"/>
-      <c r="E91" s="81" t="s">
+      <c r="C91" s="82"/>
+      <c r="D91" s="84"/>
+      <c r="E91" s="82" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="92" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A92" s="81" t="s">
+      <c r="A92" s="82" t="s">
         <v>301</v>
       </c>
-      <c r="B92" s="84" t="s">
+      <c r="B92" s="85" t="s">
         <v>293</v>
       </c>
-      <c r="C92" s="81"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="81" t="s">
+      <c r="C92" s="82"/>
+      <c r="D92" s="84"/>
+      <c r="E92" s="82" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="93" ht="48" customHeight="1" spans="1:5">
-      <c r="A93" s="81" t="s">
+      <c r="A93" s="82" t="s">
         <v>302</v>
       </c>
-      <c r="B93" s="84" t="s">
+      <c r="B93" s="85" t="s">
         <v>303</v>
       </c>
-      <c r="C93" s="81"/>
-      <c r="D93" s="83"/>
-      <c r="E93" s="81" t="s">
+      <c r="C93" s="82"/>
+      <c r="D93" s="84"/>
+      <c r="E93" s="82" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="94" ht="18.75" customHeight="1" spans="1:5">
-      <c r="A94" s="81" t="s">
+      <c r="A94" s="82" t="s">
         <v>305</v>
       </c>
-      <c r="B94" s="84" t="s">
+      <c r="B94" s="85" t="s">
         <v>293</v>
       </c>
-      <c r="C94" s="81"/>
-      <c r="D94" s="83"/>
-      <c r="E94" s="81" t="s">
+      <c r="C94" s="82"/>
+      <c r="D94" s="84"/>
+      <c r="E94" s="82" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="95" ht="64.5" customHeight="1" spans="1:5">
-      <c r="A95" s="81" t="s">
+      <c r="A95" s="82" t="s">
         <v>306</v>
       </c>
-      <c r="B95" s="84" t="s">
+      <c r="B95" s="85" t="s">
         <v>307</v>
       </c>
-      <c r="C95" s="81"/>
-      <c r="D95" s="83"/>
-      <c r="E95" s="81" t="s">
+      <c r="C95" s="82"/>
+      <c r="D95" s="84"/>
+      <c r="E95" s="82" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="96" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A96" s="81" t="s">
+      <c r="A96" s="82" t="s">
         <v>309</v>
       </c>
-      <c r="B96" s="84" t="s">
+      <c r="B96" s="85" t="s">
         <v>293</v>
       </c>
-      <c r="C96" s="81"/>
-      <c r="D96" s="83"/>
-      <c r="E96" s="81" t="s">
+      <c r="C96" s="82"/>
+      <c r="D96" s="84"/>
+      <c r="E96" s="82" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="97" ht="48.75" customHeight="1" spans="1:5">
-      <c r="A97" s="81" t="s">
+      <c r="A97" s="82" t="s">
         <v>310</v>
       </c>
-      <c r="B97" s="84" t="s">
+      <c r="B97" s="85" t="s">
         <v>311</v>
       </c>
-      <c r="C97" s="81"/>
-      <c r="D97" s="83"/>
-      <c r="E97" s="81" t="s">
+      <c r="C97" s="82"/>
+      <c r="D97" s="84"/>
+      <c r="E97" s="82" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="98" ht="49.5" customHeight="1" spans="1:5">
-      <c r="A98" s="81" t="s">
+      <c r="A98" s="82" t="s">
         <v>313</v>
       </c>
-      <c r="B98" s="84" t="s">
+      <c r="B98" s="85" t="s">
         <v>314</v>
       </c>
-      <c r="C98" s="81"/>
-      <c r="D98" s="83"/>
-      <c r="E98" s="81" t="s">
+      <c r="C98" s="82"/>
+      <c r="D98" s="84"/>
+      <c r="E98" s="82" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="99" ht="38.25" customHeight="1" spans="1:5">
-      <c r="A99" s="81" t="s">
+      <c r="A99" s="82" t="s">
         <v>315</v>
       </c>
-      <c r="B99" s="84" t="s">
+      <c r="B99" s="85" t="s">
         <v>316</v>
       </c>
-      <c r="C99" s="81"/>
-      <c r="D99" s="83"/>
-      <c r="E99" s="81" t="s">
+      <c r="C99" s="82"/>
+      <c r="D99" s="84"/>
+      <c r="E99" s="82" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="100" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A100" s="81" t="s">
+      <c r="A100" s="82" t="s">
         <v>318</v>
       </c>
-      <c r="B100" s="84" t="s">
+      <c r="B100" s="85" t="s">
         <v>319</v>
       </c>
-      <c r="C100" s="81"/>
-      <c r="D100" s="83"/>
-      <c r="E100" s="81" t="s">
+      <c r="C100" s="82"/>
+      <c r="D100" s="84"/>
+      <c r="E100" s="82" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="101" ht="48" customHeight="1" spans="1:5">
-      <c r="A101" s="81" t="s">
+      <c r="A101" s="82" t="s">
         <v>320</v>
       </c>
-      <c r="B101" s="84" t="s">
+      <c r="B101" s="85" t="s">
         <v>321</v>
       </c>
-      <c r="C101" s="81"/>
-      <c r="D101" s="83"/>
-      <c r="E101" s="81" t="s">
+      <c r="C101" s="82"/>
+      <c r="D101" s="84"/>
+      <c r="E101" s="82" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="102" ht="33" customHeight="1" spans="1:5">
-      <c r="A102" s="81" t="s">
+      <c r="A102" s="82" t="s">
         <v>323</v>
       </c>
-      <c r="B102" s="84" t="s">
+      <c r="B102" s="85" t="s">
         <v>324</v>
       </c>
-      <c r="C102" s="81"/>
-      <c r="D102" s="83"/>
-      <c r="E102" s="81" t="s">
+      <c r="C102" s="82"/>
+      <c r="D102" s="84"/>
+      <c r="E102" s="82" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="103" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A103" s="81" t="s">
+      <c r="A103" s="82" t="s">
         <v>325</v>
       </c>
-      <c r="B103" s="84" t="s">
+      <c r="B103" s="85" t="s">
         <v>326</v>
       </c>
-      <c r="C103" s="81"/>
-      <c r="D103" s="83"/>
-      <c r="E103" s="81" t="s">
+      <c r="C103" s="82"/>
+      <c r="D103" s="84"/>
+      <c r="E103" s="82" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="104" ht="46.5" customHeight="1" spans="1:5">
-      <c r="A104" s="81" t="s">
+      <c r="A104" s="82" t="s">
         <v>327</v>
       </c>
-      <c r="B104" s="84" t="s">
+      <c r="B104" s="85" t="s">
         <v>328</v>
       </c>
-      <c r="C104" s="81"/>
-      <c r="D104" s="83"/>
-      <c r="E104" s="81" t="s">
+      <c r="C104" s="82"/>
+      <c r="D104" s="84"/>
+      <c r="E104" s="82" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="105" ht="33" customHeight="1" spans="1:5">
-      <c r="A105" s="81" t="s">
+      <c r="A105" s="82" t="s">
         <v>330</v>
       </c>
-      <c r="B105" s="84" t="s">
+      <c r="B105" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="C105" s="81"/>
-      <c r="D105" s="83"/>
-      <c r="E105" s="81" t="s">
+      <c r="C105" s="82"/>
+      <c r="D105" s="84"/>
+      <c r="E105" s="82" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="106" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A106" s="81" t="s">
+      <c r="A106" s="82" t="s">
         <v>332</v>
       </c>
-      <c r="B106" s="84" t="s">
+      <c r="B106" s="85" t="s">
         <v>326</v>
       </c>
-      <c r="C106" s="81"/>
-      <c r="D106" s="83"/>
-      <c r="E106" s="81" t="s">
+      <c r="C106" s="82"/>
+      <c r="D106" s="84"/>
+      <c r="E106" s="82" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="107" ht="49.5" customHeight="1" spans="1:5">
-      <c r="A107" s="81" t="s">
+      <c r="A107" s="82" t="s">
         <v>333</v>
       </c>
-      <c r="B107" s="84" t="s">
+      <c r="B107" s="85" t="s">
         <v>334</v>
       </c>
-      <c r="C107" s="81"/>
-      <c r="D107" s="83"/>
-      <c r="E107" s="81" t="s">
+      <c r="C107" s="82"/>
+      <c r="D107" s="84"/>
+      <c r="E107" s="82" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="108" ht="36.75" customHeight="1" spans="1:5">
-      <c r="A108" s="81" t="s">
+      <c r="A108" s="82" t="s">
         <v>336</v>
       </c>
-      <c r="B108" s="84" t="s">
+      <c r="B108" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="C108" s="81"/>
-      <c r="D108" s="83"/>
-      <c r="E108" s="81" t="s">
+      <c r="C108" s="82"/>
+      <c r="D108" s="84"/>
+      <c r="E108" s="82" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="109" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A109" s="81" t="s">
+      <c r="A109" s="82" t="s">
         <v>337</v>
       </c>
-      <c r="B109" s="84" t="s">
+      <c r="B109" s="85" t="s">
         <v>326</v>
       </c>
-      <c r="C109" s="81"/>
-      <c r="D109" s="83"/>
-      <c r="E109" s="81" t="s">
+      <c r="C109" s="82"/>
+      <c r="D109" s="84"/>
+      <c r="E109" s="82" t="s">
         <v>335</v>
       </c>
     </row>
     <row r="110" ht="49.5" customHeight="1" spans="1:5">
-      <c r="A110" s="81" t="s">
+      <c r="A110" s="82" t="s">
         <v>338</v>
       </c>
-      <c r="B110" s="84" t="s">
+      <c r="B110" s="85" t="s">
         <v>339</v>
       </c>
-      <c r="C110" s="81"/>
-      <c r="D110" s="83"/>
-      <c r="E110" s="81" t="s">
+      <c r="C110" s="82"/>
+      <c r="D110" s="84"/>
+      <c r="E110" s="82" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="111" ht="33" customHeight="1" spans="1:5">
-      <c r="A111" s="81" t="s">
+      <c r="A111" s="82" t="s">
         <v>340</v>
       </c>
-      <c r="B111" s="84" t="s">
+      <c r="B111" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="C111" s="81"/>
-      <c r="D111" s="83"/>
-      <c r="E111" s="81" t="s">
+      <c r="C111" s="82"/>
+      <c r="D111" s="84"/>
+      <c r="E111" s="82" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="112" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A112" s="81" t="s">
+      <c r="A112" s="82" t="s">
         <v>341</v>
       </c>
-      <c r="B112" s="84" t="s">
+      <c r="B112" s="85" t="s">
         <v>326</v>
       </c>
-      <c r="C112" s="81"/>
-      <c r="D112" s="83"/>
-      <c r="E112" s="81" t="s">
+      <c r="C112" s="82"/>
+      <c r="D112" s="84"/>
+      <c r="E112" s="82" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="113" ht="49.5" customHeight="1" spans="1:5">
-      <c r="A113" s="81" t="s">
+      <c r="A113" s="82" t="s">
         <v>342</v>
       </c>
-      <c r="B113" s="84" t="s">
+      <c r="B113" s="85" t="s">
         <v>343</v>
       </c>
-      <c r="C113" s="81"/>
-      <c r="D113" s="83"/>
-      <c r="E113" s="81" t="s">
+      <c r="C113" s="82"/>
+      <c r="D113" s="84"/>
+      <c r="E113" s="82" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="114" ht="34.5" customHeight="1" spans="1:5">
-      <c r="A114" s="81" t="s">
+      <c r="A114" s="82" t="s">
         <v>344</v>
       </c>
-      <c r="B114" s="84" t="s">
+      <c r="B114" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="C114" s="81"/>
-      <c r="D114" s="83"/>
-      <c r="E114" s="81" t="s">
+      <c r="C114" s="82"/>
+      <c r="D114" s="84"/>
+      <c r="E114" s="82" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="115" ht="19.5" customHeight="1" spans="1:5">
-      <c r="A115" s="81" t="s">
+      <c r="A115" s="82" t="s">
         <v>345</v>
       </c>
-      <c r="B115" s="84" t="s">
+      <c r="B115" s="85" t="s">
         <v>326</v>
       </c>
-      <c r="C115" s="81"/>
-      <c r="D115" s="83"/>
-      <c r="E115" s="81" t="s">
+      <c r="C115" s="82"/>
+      <c r="D115" s="84"/>
+      <c r="E115" s="82" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="116" ht="34.5" customHeight="1" spans="1:5">
-      <c r="A116" s="81" t="s">
+      <c r="A116" s="82" t="s">
         <v>346</v>
       </c>
-      <c r="B116" s="84" t="s">
+      <c r="B116" s="85" t="s">
         <v>347</v>
       </c>
-      <c r="C116" s="81"/>
-      <c r="D116" s="83"/>
-      <c r="E116" s="81" t="s">
+      <c r="C116" s="82"/>
+      <c r="D116" s="84"/>
+      <c r="E116" s="82" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="117" ht="34.5" customHeight="1" spans="1:5">
-      <c r="A117" s="81" t="s">
+      <c r="A117" s="82" t="s">
         <v>349</v>
       </c>
-      <c r="B117" s="84" t="s">
+      <c r="B117" s="85" t="s">
         <v>95</v>
       </c>
-      <c r="C117" s="81"/>
-      <c r="D117" s="83"/>
-      <c r="E117" s="81" t="s">
+      <c r="C117" s="82"/>
+      <c r="D117" s="84"/>
+      <c r="E117" s="82" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="118" spans="1:1">
-      <c r="A118" s="93"/>
+      <c r="A118" s="94"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:B118">
@@ -7687,8 +7690,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="B238" sqref="B238"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="B242" sqref="B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11671,7 +11674,7 @@
       <c r="A242" s="46" t="s">
         <v>552</v>
       </c>
-      <c r="B242" s="48" t="s">
+      <c r="B242" s="67" t="s">
         <v>867</v>
       </c>
       <c r="C242" s="46" t="s">
@@ -11744,7 +11747,7 @@
       <c r="D246" s="46" t="s">
         <v>876</v>
       </c>
-      <c r="E246" s="67" t="s">
+      <c r="E246" s="68" t="s">
         <v>877</v>
       </c>
       <c r="F246" s="54"/>
@@ -11762,7 +11765,7 @@
       <c r="D247" s="46" t="s">
         <v>879</v>
       </c>
-      <c r="E247" s="67"/>
+      <c r="E247" s="68"/>
       <c r="F247" s="54"/>
     </row>
     <row r="248" ht="29.25" customHeight="1" spans="1:6">
@@ -11778,7 +11781,7 @@
       <c r="D248" s="46" t="s">
         <v>881</v>
       </c>
-      <c r="E248" s="67"/>
+      <c r="E248" s="68"/>
       <c r="F248" s="54"/>
     </row>
     <row r="249" ht="19.5" customHeight="1" spans="1:6">
@@ -11794,7 +11797,7 @@
       <c r="D249" s="46" t="s">
         <v>883</v>
       </c>
-      <c r="E249" s="67"/>
+      <c r="E249" s="68"/>
       <c r="F249" s="54"/>
     </row>
     <row r="250" ht="19.5" customHeight="1" spans="1:6">
@@ -11810,7 +11813,7 @@
       <c r="D250" s="46" t="s">
         <v>885</v>
       </c>
-      <c r="E250" s="67"/>
+      <c r="E250" s="68"/>
       <c r="F250" s="54"/>
     </row>
     <row r="251" ht="43.5" customHeight="1" spans="1:6">
@@ -11826,7 +11829,7 @@
       <c r="D251" s="46" t="s">
         <v>887</v>
       </c>
-      <c r="E251" s="67"/>
+      <c r="E251" s="68"/>
       <c r="F251" s="54"/>
     </row>
     <row r="252" s="41" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -12969,7 +12972,7 @@
       <c r="A321" s="46" t="s">
         <v>752</v>
       </c>
-      <c r="B321" s="68" t="s">
+      <c r="B321" s="69" t="s">
         <v>1011</v>
       </c>
       <c r="C321" s="46" t="s">
@@ -13660,7 +13663,7 @@
       <c r="B360" s="37" t="s">
         <v>1096</v>
       </c>
-      <c r="C360" s="69">
+      <c r="C360" s="70">
         <v>45313</v>
       </c>
       <c r="D360" s="46" t="s">
@@ -13676,7 +13679,7 @@
       <c r="B361" s="37" t="s">
         <v>1098</v>
       </c>
-      <c r="C361" s="70">
+      <c r="C361" s="71">
         <v>45344</v>
       </c>
       <c r="D361" s="46" t="s">
@@ -13692,7 +13695,7 @@
       <c r="B362" s="37" t="s">
         <v>1100</v>
       </c>
-      <c r="C362" s="70">
+      <c r="C362" s="71">
         <v>45344</v>
       </c>
       <c r="D362" s="46" t="s">
@@ -13708,7 +13711,7 @@
       <c r="B363" s="37" t="s">
         <v>1102</v>
       </c>
-      <c r="C363" s="70">
+      <c r="C363" s="71">
         <v>45344</v>
       </c>
       <c r="D363" s="46" t="s">
@@ -13724,7 +13727,7 @@
       <c r="B364" s="37" t="s">
         <v>1104</v>
       </c>
-      <c r="C364" s="70">
+      <c r="C364" s="71">
         <v>45344</v>
       </c>
       <c r="D364" s="46" t="s">
@@ -13740,7 +13743,7 @@
       <c r="B365" s="37" t="s">
         <v>1106</v>
       </c>
-      <c r="C365" s="70">
+      <c r="C365" s="71">
         <v>45344</v>
       </c>
       <c r="D365" s="46" t="s">
@@ -13756,7 +13759,7 @@
       <c r="B366" s="37" t="s">
         <v>1108</v>
       </c>
-      <c r="C366" s="70">
+      <c r="C366" s="71">
         <v>45344</v>
       </c>
       <c r="D366" s="46" t="s">
@@ -13772,7 +13775,7 @@
       <c r="B367" s="37" t="s">
         <v>1110</v>
       </c>
-      <c r="C367" s="70">
+      <c r="C367" s="71">
         <v>45344</v>
       </c>
       <c r="D367" s="46" t="s">
@@ -13788,7 +13791,7 @@
       <c r="B368" s="37" t="s">
         <v>1112</v>
       </c>
-      <c r="C368" s="70">
+      <c r="C368" s="71">
         <v>45344</v>
       </c>
       <c r="D368" s="46" t="s">
@@ -13804,7 +13807,7 @@
       <c r="B369" s="37" t="s">
         <v>1114</v>
       </c>
-      <c r="C369" s="70">
+      <c r="C369" s="71">
         <v>45344</v>
       </c>
       <c r="D369" s="46" t="s">
@@ -13820,7 +13823,7 @@
       <c r="B370" s="37" t="s">
         <v>1116</v>
       </c>
-      <c r="C370" s="70">
+      <c r="C370" s="71">
         <v>45344</v>
       </c>
       <c r="D370" s="46" t="s">
@@ -13836,7 +13839,7 @@
       <c r="B371" s="37" t="s">
         <v>1118</v>
       </c>
-      <c r="C371" s="70">
+      <c r="C371" s="71">
         <v>45344</v>
       </c>
       <c r="D371" s="46" t="s">
@@ -13852,7 +13855,7 @@
       <c r="B372" s="37" t="s">
         <v>1120</v>
       </c>
-      <c r="C372" s="70">
+      <c r="C372" s="71">
         <v>45344</v>
       </c>
       <c r="D372" s="46" t="s">
@@ -13868,7 +13871,7 @@
       <c r="B373" s="37" t="s">
         <v>1122</v>
       </c>
-      <c r="C373" s="70">
+      <c r="C373" s="71">
         <v>45344</v>
       </c>
       <c r="D373" s="46" t="s">

</xml_diff>

<commit_message>
new SOP: SOP Evaluasi Ketersediaan Obat terhadap Formularium Puskesmas
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -4461,12 +4461,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -4549,32 +4549,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4582,7 +4564,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4595,28 +4577,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -4639,6 +4609,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -4654,23 +4638,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4684,6 +4668,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -4692,14 +4684,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4762,25 +4762,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4798,7 +4786,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4810,13 +4804,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4828,7 +4858,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4840,7 +4888,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4852,31 +4906,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4888,61 +4930,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5050,21 +5050,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -5138,141 +5123,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="35" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="39" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5437,12 +5437,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5451,10 +5451,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5518,7 +5518,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7691,7 +7691,7 @@
   <dimension ref="A1:G373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+      <selection activeCell="B230" sqref="B230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11478,7 +11478,7 @@
       <c r="A230" s="46" t="s">
         <v>525</v>
       </c>
-      <c r="B230" s="48" t="s">
+      <c r="B230" s="65" t="s">
         <v>841</v>
       </c>
       <c r="C230" s="46" t="s">
@@ -11574,7 +11574,7 @@
       <c r="A236" s="46" t="s">
         <v>539</v>
       </c>
-      <c r="B236" s="65" t="s">
+      <c r="B236" s="66" t="s">
         <v>853</v>
       </c>
       <c r="C236" s="46" t="s">
@@ -11590,7 +11590,7 @@
       <c r="A237" s="46" t="s">
         <v>541</v>
       </c>
-      <c r="B237" s="65" t="s">
+      <c r="B237" s="66" t="s">
         <v>855</v>
       </c>
       <c r="C237" s="46" t="s">
@@ -11606,7 +11606,7 @@
       <c r="A238" s="46" t="s">
         <v>543</v>
       </c>
-      <c r="B238" s="65" t="s">
+      <c r="B238" s="66" t="s">
         <v>857</v>
       </c>
       <c r="C238" s="46" t="s">
@@ -11638,7 +11638,7 @@
       <c r="A240" s="46" t="s">
         <v>547</v>
       </c>
-      <c r="B240" s="66" t="s">
+      <c r="B240" s="67" t="s">
         <v>861</v>
       </c>
       <c r="C240" s="46" t="s">
@@ -11656,7 +11656,7 @@
       <c r="A241" s="46" t="s">
         <v>549</v>
       </c>
-      <c r="B241" s="66" t="s">
+      <c r="B241" s="67" t="s">
         <v>864</v>
       </c>
       <c r="C241" s="46" t="s">
@@ -11674,7 +11674,7 @@
       <c r="A242" s="46" t="s">
         <v>552</v>
       </c>
-      <c r="B242" s="67" t="s">
+      <c r="B242" s="65" t="s">
         <v>867</v>
       </c>
       <c r="C242" s="46" t="s">

</xml_diff>

<commit_message>
new SOP: EP07 Kesesuaian Peresepan, tambah sampul EP06
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3012" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3015" uniqueCount="1475">
   <si>
     <t>PENOMORAN SK</t>
   </si>
@@ -2493,6 +2493,9 @@
     <t>350</t>
   </si>
   <si>
+    <t>uploaded with sampul</t>
+  </si>
+  <si>
     <t>SOP pemantauan/ monitoring obat gawat darurat secara berkala</t>
   </si>
   <si>
@@ -2557,9 +2560,6 @@
   </si>
   <si>
     <t>361</t>
-  </si>
-  <si>
-    <t>uploaded with sampul</t>
   </si>
   <si>
     <t>SOP Pengelolaan Obat Kadaluarsa</t>
@@ -4464,12 +4464,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -4571,24 +4571,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4602,41 +4593,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4648,16 +4609,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4678,23 +4631,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4709,6 +4671,44 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4771,37 +4771,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4819,19 +4807,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4843,31 +4861,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4879,25 +4921,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4909,43 +4945,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5050,36 +5050,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -5109,11 +5083,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5133,151 +5113,171 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="25" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5461,10 +5461,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5528,7 +5528,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7700,8 +7700,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="F231" sqref="F231"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="C234" sqref="C234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11320,38 +11320,42 @@
       <c r="E219" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="F219" s="54"/>
+      <c r="F219" s="68" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="220" ht="19.5" customHeight="1" spans="1:6">
       <c r="A220" s="46" t="s">
         <v>505</v>
       </c>
       <c r="B220" s="63" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="C220" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D220" s="46" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="E220" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="F220" s="54"/>
+      <c r="F220" s="68" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="221" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A221" s="46" t="s">
         <v>507</v>
       </c>
       <c r="B221" s="64" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C221" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D221" s="46" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="E221" s="57"/>
       <c r="F221" s="62"/>
@@ -11361,13 +11365,13 @@
         <v>509</v>
       </c>
       <c r="B222" s="64" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C222" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D222" s="46" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="E222" s="57"/>
       <c r="F222" s="62"/>
@@ -11377,13 +11381,13 @@
         <v>511</v>
       </c>
       <c r="B223" s="64" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="C223" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D223" s="46" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="E223" s="57"/>
       <c r="F223" s="62"/>
@@ -11393,13 +11397,13 @@
         <v>513</v>
       </c>
       <c r="B224" s="64" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C224" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D224" s="46" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="E224" s="57"/>
       <c r="F224" s="62"/>
@@ -11409,13 +11413,13 @@
         <v>515</v>
       </c>
       <c r="B225" s="64" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="C225" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D225" s="46" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E225" s="57"/>
       <c r="F225" s="62"/>
@@ -11425,13 +11429,13 @@
         <v>517</v>
       </c>
       <c r="B226" s="64" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="C226" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D226" s="46" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E226" s="57"/>
       <c r="F226" s="62"/>
@@ -11441,13 +11445,13 @@
         <v>519</v>
       </c>
       <c r="B227" s="64" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C227" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D227" s="46" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E227" s="57"/>
       <c r="F227" s="62"/>
@@ -11457,13 +11461,13 @@
         <v>521</v>
       </c>
       <c r="B228" s="64" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C228" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D228" s="46" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E228" s="57"/>
       <c r="F228" s="62"/>
@@ -11473,13 +11477,13 @@
         <v>523</v>
       </c>
       <c r="B229" s="64" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C229" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D229" s="46" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E229" s="57"/>
       <c r="F229" s="62"/>
@@ -11489,17 +11493,17 @@
         <v>525</v>
       </c>
       <c r="B230" s="65" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="C230" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D230" s="46" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="E230" s="57"/>
       <c r="F230" s="68" t="s">
-        <v>843</v>
+        <v>821</v>
       </c>
     </row>
     <row r="231" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -11718,7 +11722,7 @@
       <c r="A244" s="46" t="s">
         <v>556</v>
       </c>
-      <c r="B244" s="48" t="s">
+      <c r="B244" s="65" t="s">
         <v>872</v>
       </c>
       <c r="C244" s="46" t="s">
@@ -11728,7 +11732,9 @@
         <v>873</v>
       </c>
       <c r="E244" s="57"/>
-      <c r="F244" s="62"/>
+      <c r="F244" s="68" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="245" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A245" s="46" t="s">
@@ -13606,7 +13612,7 @@
     </row>
     <row r="356" ht="19.5" customHeight="1" spans="1:6">
       <c r="A356" s="46" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B356" s="37" t="s">
         <v>1088</v>
@@ -13622,7 +13628,7 @@
     </row>
     <row r="357" ht="19.5" customHeight="1" spans="1:6">
       <c r="A357" s="46" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B357" s="37" t="s">
         <v>1090</v>
@@ -13638,7 +13644,7 @@
     </row>
     <row r="358" ht="19.5" customHeight="1" spans="1:6">
       <c r="A358" s="46" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B358" s="37" t="s">
         <v>1092</v>
@@ -13654,7 +13660,7 @@
     </row>
     <row r="359" ht="19.5" customHeight="1" spans="1:6">
       <c r="A359" s="46" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B359" s="37" t="s">
         <v>1094</v>
@@ -13670,7 +13676,7 @@
     </row>
     <row r="360" ht="19.5" customHeight="1" spans="1:6">
       <c r="A360" s="46" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B360" s="37" t="s">
         <v>1097</v>
@@ -13686,7 +13692,7 @@
     </row>
     <row r="361" ht="19.5" customHeight="1" spans="1:6">
       <c r="A361" s="46" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B361" s="37" t="s">
         <v>1099</v>
@@ -13702,7 +13708,7 @@
     </row>
     <row r="362" ht="19.5" customHeight="1" spans="1:6">
       <c r="A362" s="46" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B362" s="37" t="s">
         <v>1101</v>
@@ -13718,7 +13724,7 @@
     </row>
     <row r="363" ht="19.5" customHeight="1" spans="1:6">
       <c r="A363" s="46" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B363" s="37" t="s">
         <v>1103</v>
@@ -13734,7 +13740,7 @@
     </row>
     <row r="364" ht="19.5" customHeight="1" spans="1:6">
       <c r="A364" s="46" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B364" s="37" t="s">
         <v>1105</v>
@@ -13750,7 +13756,7 @@
     </row>
     <row r="365" ht="19.5" customHeight="1" spans="1:6">
       <c r="A365" s="46" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B365" s="37" t="s">
         <v>1107</v>
@@ -13766,7 +13772,7 @@
     </row>
     <row r="366" ht="19.5" customHeight="1" spans="1:6">
       <c r="A366" s="46" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B366" s="37" t="s">
         <v>1109</v>

</xml_diff>

<commit_message>
upload EP06 Penyediaan dan Penyimpanan Obat emergensi
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -2502,13 +2502,13 @@
     <t>350</t>
   </si>
   <si>
+    <t>SOP pemantauan/ monitoring obat gawat darurat secara berkala</t>
+  </si>
+  <si>
+    <t>351</t>
+  </si>
+  <si>
     <t>uploaded with sampul</t>
-  </si>
-  <si>
-    <t>SOP pemantauan/ monitoring obat gawat darurat secara berkala</t>
-  </si>
-  <si>
-    <t>351</t>
   </si>
   <si>
     <t>SOP Formularium Puskesmas</t>
@@ -4476,12 +4476,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -4583,19 +4583,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4607,16 +4606,16 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4630,24 +4629,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4660,9 +4652,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4678,28 +4705,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4712,17 +4718,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4783,7 +4783,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4795,13 +4795,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4813,13 +4837,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4831,19 +4849,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4855,7 +4909,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4867,25 +4933,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4897,73 +4963,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5062,69 +5062,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -5151,6 +5088,69 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -5162,131 +5162,131 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7713,8 +7713,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="G218" sqref="G218"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="G219" sqref="G219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11327,7 +11327,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="219" ht="19.5" customHeight="1" spans="1:6">
+    <row r="219" ht="19.5" customHeight="1" spans="1:7">
       <c r="A219" s="46" t="s">
         <v>503</v>
       </c>
@@ -11343,8 +11343,9 @@
       <c r="E219" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="F219" s="69" t="s">
-        <v>824</v>
+      <c r="F219" s="69"/>
+      <c r="G219" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="220" ht="19.5" customHeight="1" spans="1:6">
@@ -11352,19 +11353,19 @@
         <v>505</v>
       </c>
       <c r="B220" s="63" t="s">
+        <v>824</v>
+      </c>
+      <c r="C220" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D220" s="46" t="s">
         <v>825</v>
-      </c>
-      <c r="C220" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D220" s="46" t="s">
-        <v>826</v>
       </c>
       <c r="E220" s="46" t="s">
         <v>146</v>
       </c>
       <c r="F220" s="69" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="221" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -11526,7 +11527,7 @@
       </c>
       <c r="E230" s="57"/>
       <c r="F230" s="69" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="231" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -11758,7 +11759,7 @@
       </c>
       <c r="E244" s="57"/>
       <c r="F244" s="69" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="245" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -13637,7 +13638,7 @@
     </row>
     <row r="356" ht="19.5" customHeight="1" spans="1:6">
       <c r="A356" s="46" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B356" s="37" t="s">
         <v>1092</v>

</xml_diff>

<commit_message>
upload EP06 Monitoring obat emergensi
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -2508,67 +2508,67 @@
     <t>351</t>
   </si>
   <si>
+    <t>SOP Formularium Puskesmas</t>
+  </si>
+  <si>
+    <t>352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP Perencanaan </t>
+  </si>
+  <si>
+    <t>353</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP Permintaan dan Pengadaan </t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP Permintaan Internal </t>
+  </si>
+  <si>
+    <t>355</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP Penerimaan </t>
+  </si>
+  <si>
+    <t>356</t>
+  </si>
+  <si>
+    <t>SOP Penyimpanan</t>
+  </si>
+  <si>
+    <t>357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP Pendistribusian </t>
+  </si>
+  <si>
+    <t>358</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP Pengendalian </t>
+  </si>
+  <si>
+    <t>359</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOP Pencatatan Pelaporan Farmasi </t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>SOP Evaluasi Ketersediaan Obat Terhadap Formularium</t>
+  </si>
+  <si>
+    <t>361</t>
+  </si>
+  <si>
     <t>uploaded with sampul</t>
-  </si>
-  <si>
-    <t>SOP Formularium Puskesmas</t>
-  </si>
-  <si>
-    <t>352</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP Perencanaan </t>
-  </si>
-  <si>
-    <t>353</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP Permintaan dan Pengadaan </t>
-  </si>
-  <si>
-    <t>354</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP Permintaan Internal </t>
-  </si>
-  <si>
-    <t>355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP Penerimaan </t>
-  </si>
-  <si>
-    <t>356</t>
-  </si>
-  <si>
-    <t>SOP Penyimpanan</t>
-  </si>
-  <si>
-    <t>357</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP Pendistribusian </t>
-  </si>
-  <si>
-    <t>358</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP Pengendalian </t>
-  </si>
-  <si>
-    <t>359</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOP Pencatatan Pelaporan Farmasi </t>
-  </si>
-  <si>
-    <t>360</t>
-  </si>
-  <si>
-    <t>SOP Evaluasi Ketersediaan Obat Terhadap Formularium</t>
-  </si>
-  <si>
-    <t>361</t>
   </si>
   <si>
     <t>SOP Pengelolaan Obat Kadaluarsa</t>
@@ -4476,11 +4476,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="35">
@@ -4578,23 +4578,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4605,9 +4593,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4616,6 +4624,42 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4631,15 +4675,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4652,77 +4718,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -4783,7 +4783,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4795,19 +4807,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4825,7 +4921,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4837,133 +4957,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5064,41 +5064,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5114,6 +5082,24 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5135,164 +5121,178 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="38" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="32" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -7714,7 +7714,7 @@
   <dimension ref="A1:G373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="G219" sqref="G219"/>
+      <selection activeCell="G220" sqref="G220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11348,7 +11348,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="220" ht="19.5" customHeight="1" spans="1:6">
+    <row r="220" ht="19.5" customHeight="1" spans="1:7">
       <c r="A220" s="46" t="s">
         <v>505</v>
       </c>
@@ -11364,8 +11364,9 @@
       <c r="E220" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="F220" s="69" t="s">
-        <v>826</v>
+      <c r="F220" s="69"/>
+      <c r="G220" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="221" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -11373,13 +11374,13 @@
         <v>507</v>
       </c>
       <c r="B221" s="64" t="s">
+        <v>826</v>
+      </c>
+      <c r="C221" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D221" s="46" t="s">
         <v>827</v>
-      </c>
-      <c r="C221" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D221" s="46" t="s">
-        <v>828</v>
       </c>
       <c r="E221" s="57"/>
       <c r="F221" s="62"/>
@@ -11389,13 +11390,13 @@
         <v>509</v>
       </c>
       <c r="B222" s="64" t="s">
+        <v>828</v>
+      </c>
+      <c r="C222" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D222" s="46" t="s">
         <v>829</v>
-      </c>
-      <c r="C222" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D222" s="46" t="s">
-        <v>830</v>
       </c>
       <c r="E222" s="57"/>
       <c r="F222" s="62"/>
@@ -11405,13 +11406,13 @@
         <v>511</v>
       </c>
       <c r="B223" s="64" t="s">
+        <v>830</v>
+      </c>
+      <c r="C223" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D223" s="46" t="s">
         <v>831</v>
-      </c>
-      <c r="C223" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D223" s="46" t="s">
-        <v>832</v>
       </c>
       <c r="E223" s="57"/>
       <c r="F223" s="62"/>
@@ -11421,13 +11422,13 @@
         <v>513</v>
       </c>
       <c r="B224" s="64" t="s">
+        <v>832</v>
+      </c>
+      <c r="C224" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D224" s="46" t="s">
         <v>833</v>
-      </c>
-      <c r="C224" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D224" s="46" t="s">
-        <v>834</v>
       </c>
       <c r="E224" s="57"/>
       <c r="F224" s="62"/>
@@ -11437,13 +11438,13 @@
         <v>515</v>
       </c>
       <c r="B225" s="64" t="s">
+        <v>834</v>
+      </c>
+      <c r="C225" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D225" s="46" t="s">
         <v>835</v>
-      </c>
-      <c r="C225" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D225" s="46" t="s">
-        <v>836</v>
       </c>
       <c r="E225" s="57"/>
       <c r="F225" s="62"/>
@@ -11453,13 +11454,13 @@
         <v>517</v>
       </c>
       <c r="B226" s="64" t="s">
+        <v>836</v>
+      </c>
+      <c r="C226" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D226" s="46" t="s">
         <v>837</v>
-      </c>
-      <c r="C226" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D226" s="46" t="s">
-        <v>838</v>
       </c>
       <c r="E226" s="57"/>
       <c r="F226" s="62"/>
@@ -11469,13 +11470,13 @@
         <v>519</v>
       </c>
       <c r="B227" s="64" t="s">
+        <v>838</v>
+      </c>
+      <c r="C227" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D227" s="46" t="s">
         <v>839</v>
-      </c>
-      <c r="C227" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D227" s="46" t="s">
-        <v>840</v>
       </c>
       <c r="E227" s="57"/>
       <c r="F227" s="62"/>
@@ -11485,13 +11486,13 @@
         <v>521</v>
       </c>
       <c r="B228" s="64" t="s">
+        <v>840</v>
+      </c>
+      <c r="C228" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D228" s="46" t="s">
         <v>841</v>
-      </c>
-      <c r="C228" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D228" s="46" t="s">
-        <v>842</v>
       </c>
       <c r="E228" s="57"/>
       <c r="F228" s="62"/>
@@ -11501,13 +11502,13 @@
         <v>523</v>
       </c>
       <c r="B229" s="64" t="s">
+        <v>842</v>
+      </c>
+      <c r="C229" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D229" s="46" t="s">
         <v>843</v>
-      </c>
-      <c r="C229" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D229" s="46" t="s">
-        <v>844</v>
       </c>
       <c r="E229" s="57"/>
       <c r="F229" s="62"/>
@@ -11517,17 +11518,17 @@
         <v>525</v>
       </c>
       <c r="B230" s="65" t="s">
+        <v>844</v>
+      </c>
+      <c r="C230" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="D230" s="46" t="s">
         <v>845</v>
-      </c>
-      <c r="C230" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="D230" s="46" t="s">
-        <v>846</v>
       </c>
       <c r="E230" s="57"/>
       <c r="F230" s="69" t="s">
-        <v>826</v>
+        <v>846</v>
       </c>
     </row>
     <row r="231" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -11759,7 +11760,7 @@
       </c>
       <c r="E244" s="57"/>
       <c r="F244" s="69" t="s">
-        <v>826</v>
+        <v>846</v>
       </c>
     </row>
     <row r="245" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -13654,7 +13655,7 @@
     </row>
     <row r="357" ht="19.5" customHeight="1" spans="1:6">
       <c r="A357" s="46" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B357" s="37" t="s">
         <v>1094</v>
@@ -13670,7 +13671,7 @@
     </row>
     <row r="358" ht="19.5" customHeight="1" spans="1:6">
       <c r="A358" s="46" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="B358" s="37" t="s">
         <v>1096</v>
@@ -13686,7 +13687,7 @@
     </row>
     <row r="359" ht="19.5" customHeight="1" spans="1:6">
       <c r="A359" s="46" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B359" s="37" t="s">
         <v>1098</v>
@@ -13702,7 +13703,7 @@
     </row>
     <row r="360" ht="19.5" customHeight="1" spans="1:6">
       <c r="A360" s="46" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="B360" s="37" t="s">
         <v>1101</v>
@@ -13718,7 +13719,7 @@
     </row>
     <row r="361" ht="19.5" customHeight="1" spans="1:6">
       <c r="A361" s="46" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B361" s="37" t="s">
         <v>1103</v>
@@ -13734,7 +13735,7 @@
     </row>
     <row r="362" ht="19.5" customHeight="1" spans="1:6">
       <c r="A362" s="46" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="B362" s="37" t="s">
         <v>1105</v>
@@ -13750,7 +13751,7 @@
     </row>
     <row r="363" ht="19.5" customHeight="1" spans="1:6">
       <c r="A363" s="46" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B363" s="37" t="s">
         <v>1107</v>
@@ -13766,7 +13767,7 @@
     </row>
     <row r="364" ht="19.5" customHeight="1" spans="1:6">
       <c r="A364" s="46" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="B364" s="37" t="s">
         <v>1109</v>
@@ -13782,7 +13783,7 @@
     </row>
     <row r="365" ht="19.5" customHeight="1" spans="1:6">
       <c r="A365" s="46" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="B365" s="37" t="s">
         <v>1111</v>
@@ -13798,7 +13799,7 @@
     </row>
     <row r="366" ht="19.5" customHeight="1" spans="1:6">
       <c r="A366" s="46" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B366" s="37" t="s">
         <v>1113</v>

</xml_diff>

<commit_message>
done upload all SOP EP03
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3020" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="1478">
   <si>
     <t>PENOMORAN SK</t>
   </si>
@@ -2478,6 +2478,9 @@
     <t>347</t>
   </si>
   <si>
+    <t>upload tanpa sampul</t>
+  </si>
+  <si>
     <t>SOP kajian resep dan pemberian obat</t>
   </si>
   <si>
@@ -2485,9 +2488,6 @@
   </si>
   <si>
     <t>dibagi 2 a dan b EP04</t>
-  </si>
-  <si>
-    <t>upload tanpa sampul</t>
   </si>
   <si>
     <t>SOP pemberian informasi obat (PIO)</t>
@@ -4473,12 +4473,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
+    <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-409]d\-mmm\-yy"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -4567,18 +4567,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -4587,9 +4575,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4604,13 +4627,57 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -4627,7 +4694,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4641,20 +4708,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -4664,60 +4717,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4780,43 +4780,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4834,13 +4804,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4852,7 +4822,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4864,7 +4834,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4876,13 +4846,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4906,7 +4870,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4918,13 +4936,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4936,31 +4954,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5074,6 +5074,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -5113,6 +5122,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -5131,166 +5151,146 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5471,10 +5471,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5538,7 +5538,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7710,8 +7710,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="G230" sqref="G230"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11262,7 +11262,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="216" ht="19.5" customHeight="1" spans="1:6">
+    <row r="216" ht="19.5" customHeight="1" spans="1:7">
       <c r="A216" s="46" t="s">
         <v>497</v>
       </c>
@@ -11279,28 +11279,31 @@
         <v>146</v>
       </c>
       <c r="F216" s="54"/>
+      <c r="G216" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="217" ht="19.5" customHeight="1" spans="1:7">
       <c r="A217" s="46" t="s">
         <v>499</v>
       </c>
       <c r="B217" s="63" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C217" s="46" t="s">
         <v>195</v>
       </c>
       <c r="D217" s="46" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="E217" s="46" t="s">
         <v>146</v>
       </c>
       <c r="F217" s="68" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="G217" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="218" ht="19.5" customHeight="1" spans="1:7">
@@ -11321,7 +11324,7 @@
       </c>
       <c r="F218" s="54"/>
       <c r="G218" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="219" ht="19.5" customHeight="1" spans="1:7">
@@ -11342,7 +11345,7 @@
       </c>
       <c r="F219" s="69"/>
       <c r="G219" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="220" ht="19.5" customHeight="1" spans="1:7">
@@ -11363,7 +11366,7 @@
       </c>
       <c r="F220" s="69"/>
       <c r="G220" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="221" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -11526,7 +11529,7 @@
       <c r="E230" s="57"/>
       <c r="F230" s="69"/>
       <c r="G230" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="231" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -11609,7 +11612,7 @@
       <c r="E235" s="57"/>
       <c r="F235" s="62"/>
     </row>
-    <row r="236" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="236" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A236" s="46" t="s">
         <v>539</v>
       </c>
@@ -11624,8 +11627,11 @@
       </c>
       <c r="E236" s="57"/>
       <c r="F236" s="62"/>
-    </row>
-    <row r="237" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+      <c r="G236" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="237" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A237" s="46" t="s">
         <v>541</v>
       </c>
@@ -11640,8 +11646,11 @@
       </c>
       <c r="E237" s="57"/>
       <c r="F237" s="62"/>
-    </row>
-    <row r="238" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+      <c r="G237" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="238" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A238" s="46" t="s">
         <v>543</v>
       </c>
@@ -11656,6 +11665,9 @@
       </c>
       <c r="E238" s="57"/>
       <c r="F238" s="62"/>
+      <c r="G238" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="239" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A239" s="46" t="s">
@@ -11759,7 +11771,7 @@
       <c r="E244" s="57"/>
       <c r="F244" s="69"/>
       <c r="G244" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
     </row>
     <row r="245" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
@@ -13584,7 +13596,7 @@
     </row>
     <row r="353" ht="19.5" customHeight="1" spans="1:6">
       <c r="A353" s="46" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B353" s="37" t="s">
         <v>1084</v>

</xml_diff>

<commit_message>
ongoing upload EP 02
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3029" uniqueCount="1478">
   <si>
     <t>PENOMORAN SK</t>
   </si>
@@ -4567,28 +4567,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -4603,18 +4588,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4626,17 +4618,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4649,29 +4647,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4694,7 +4672,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4708,16 +4701,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4780,7 +4780,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4792,7 +4888,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4804,121 +4942,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4930,37 +4954,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5059,17 +5059,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5098,10 +5092,42 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -5124,32 +5150,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -5159,138 +5159,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7710,8 +7710,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="G216" sqref="G216"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="G228" sqref="G228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11385,7 +11385,7 @@
       <c r="E221" s="57"/>
       <c r="F221" s="62"/>
     </row>
-    <row r="222" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="222" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A222" s="46" t="s">
         <v>509</v>
       </c>
@@ -11400,6 +11400,9 @@
       </c>
       <c r="E222" s="57"/>
       <c r="F222" s="62"/>
+      <c r="G222" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="223" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A223" s="46" t="s">
@@ -11417,7 +11420,7 @@
       <c r="E223" s="57"/>
       <c r="F223" s="62"/>
     </row>
-    <row r="224" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="224" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A224" s="46" t="s">
         <v>513</v>
       </c>
@@ -11432,8 +11435,11 @@
       </c>
       <c r="E224" s="57"/>
       <c r="F224" s="62"/>
-    </row>
-    <row r="225" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+      <c r="G224" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="225" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A225" s="46" t="s">
         <v>515</v>
       </c>
@@ -11448,6 +11454,9 @@
       </c>
       <c r="E225" s="57"/>
       <c r="F225" s="62"/>
+      <c r="G225" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="226" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A226" s="46" t="s">
@@ -11481,7 +11490,7 @@
       <c r="E227" s="57"/>
       <c r="F227" s="62"/>
     </row>
-    <row r="228" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="228" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A228" s="46" t="s">
         <v>521</v>
       </c>
@@ -11496,6 +11505,9 @@
       </c>
       <c r="E228" s="57"/>
       <c r="F228" s="62"/>
+      <c r="G228" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="229" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A229" s="46" t="s">
@@ -11580,7 +11592,7 @@
       <c r="E233" s="57"/>
       <c r="F233" s="62"/>
     </row>
-    <row r="234" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="234" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A234" s="46" t="s">
         <v>534</v>
       </c>
@@ -11595,6 +11607,9 @@
       </c>
       <c r="E234" s="57"/>
       <c r="F234" s="62"/>
+      <c r="G234" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="235" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A235" s="46" t="s">

</xml_diff>

<commit_message>
upload All SOP EP02 selesai
</commit_message>
<xml_diff>
--- a/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
+++ b/other/URUTAN SK SOP PEDOMAN KAK NEW-1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3029" uniqueCount="1478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="1478">
   <si>
     <t>PENOMORAN SK</t>
   </si>
@@ -4475,10 +4475,10 @@
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm\-yy"/>
     <numFmt numFmtId="177" formatCode="[$-421]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -4567,54 +4567,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4634,68 +4611,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4716,8 +4632,92 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4780,7 +4780,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4792,175 +4960,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5059,11 +5059,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5073,6 +5079,17 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5088,21 +5105,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5124,10 +5126,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -5159,138 +5159,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="27" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7710,8 +7710,8 @@
   <sheetPr/>
   <dimension ref="A1:G373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="G228" sqref="G228"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" topLeftCell="A213" workbookViewId="0">
+      <selection activeCell="G231" sqref="G231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -11404,7 +11404,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="223" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="223" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A223" s="46" t="s">
         <v>511</v>
       </c>
@@ -11419,6 +11419,9 @@
       </c>
       <c r="E223" s="57"/>
       <c r="F223" s="62"/>
+      <c r="G223" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="224" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A224" s="46" t="s">
@@ -11509,7 +11512,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="229" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="229" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A229" s="46" t="s">
         <v>523</v>
       </c>
@@ -11524,6 +11527,9 @@
       </c>
       <c r="E229" s="57"/>
       <c r="F229" s="62"/>
+      <c r="G229" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="230" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A230" s="46" t="s">
@@ -11544,7 +11550,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="231" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="231" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A231" s="46" t="s">
         <v>527</v>
       </c>
@@ -11559,8 +11565,11 @@
       </c>
       <c r="E231" s="57"/>
       <c r="F231" s="62"/>
-    </row>
-    <row r="232" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+      <c r="G231" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="232" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A232" s="46" t="s">
         <v>529</v>
       </c>
@@ -11575,8 +11584,11 @@
       </c>
       <c r="E232" s="57"/>
       <c r="F232" s="62"/>
-    </row>
-    <row r="233" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+      <c r="G232" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="233" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A233" s="46" t="s">
         <v>531</v>
       </c>
@@ -11591,6 +11603,9 @@
       </c>
       <c r="E233" s="57"/>
       <c r="F233" s="62"/>
+      <c r="G233" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="234" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A234" s="46" t="s">
@@ -11736,7 +11751,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="242" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="242" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A242" s="46" t="s">
         <v>552</v>
       </c>
@@ -11751,6 +11766,9 @@
       </c>
       <c r="E242" s="57"/>
       <c r="F242" s="62"/>
+      <c r="G242" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="243" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A243" s="46" t="s">
@@ -11789,7 +11807,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="245" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:6">
+    <row r="245" s="40" customFormat="1" ht="19.5" customHeight="1" spans="1:7">
       <c r="A245" s="46" t="s">
         <v>558</v>
       </c>
@@ -11804,6 +11822,9 @@
       </c>
       <c r="E245" s="57"/>
       <c r="F245" s="62"/>
+      <c r="G245" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="246" ht="29.25" customHeight="1" spans="1:6">
       <c r="A246" s="46" t="s">

</xml_diff>